<commit_message>
cleanup.py: phone numbers and emails complete
</commit_message>
<xml_diff>
--- a/test_files/example2.xlsx
+++ b/test_files/example2.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sydneyfowler/Desktop/CS3030/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16E8C2B-7AE0-7F45-BA66-A877DA86B1F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700" xr2:uid="{02FD7F75-EE41-F445-859C-8D52CF1904CF}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -243,9 +248,6 @@
     <t>example288@gmail.com</t>
   </si>
   <si>
-    <t>example@example.comn</t>
-  </si>
-  <si>
     <t>example@yaho.com</t>
   </si>
   <si>
@@ -273,16 +275,19 @@
     <t>65example@example.edu</t>
   </si>
   <si>
-    <t>example24@example.org</t>
-  </si>
-  <si>
     <t>exampleFFDE3@example.html</t>
+  </si>
+  <si>
+    <t>example@example.comn, example2@example.com</t>
+  </si>
+  <si>
+    <t>John Smith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -649,11 +654,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA019674-5A8D-844F-9B09-D6BFD3667472}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,7 +667,7 @@
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="43.1640625" customWidth="1"/>
     <col min="6" max="6" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -740,7 +745,7 @@
         <v>31056</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
@@ -760,7 +765,7 @@
         <v>34647</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
         <v>57</v>
@@ -780,7 +785,7 @@
         <v>48</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
         <v>58</v>
@@ -800,7 +805,7 @@
         <v>31056</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
         <v>59</v>
@@ -820,7 +825,7 @@
         <v>49</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
         <v>60</v>
@@ -840,7 +845,7 @@
         <v>34981</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" t="s">
         <v>62</v>
@@ -860,7 +865,7 @@
         <v>36892</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
         <v>63</v>
@@ -880,7 +885,7 @@
         <v>34489</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" t="s">
         <v>64</v>
@@ -900,7 +905,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>65</v>
@@ -920,7 +925,7 @@
         <v>51</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
         <v>66</v>
@@ -939,8 +944,8 @@
       <c r="D14" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>80</v>
+      <c r="E14" t="s">
+        <v>81</v>
       </c>
       <c r="F14" t="s">
         <v>55</v>
@@ -960,7 +965,7 @@
         <v>28216</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
         <v>67</v>
@@ -968,20 +973,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{160D9514-1F17-7A48-8DD6-58C3333AF13B}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{289C2835-516A-084C-AE93-EFF7E73055A5}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{A2DA9D3F-C211-AE4A-9E9D-AF87970FEEA3}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{DB5DCE76-CE34-5544-9F22-8171E0E11A93}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{75B1EF54-E7F8-F749-AEE2-2160EE85954F}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{ABF21734-FD9F-5644-9FA0-39C8CE869F4F}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{69B31341-8A96-794B-A650-03B9A3A502BC}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{021E4977-0D35-7C46-A2A8-0A5AF9DD0A5E}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{6CBE045B-D8FB-2049-A86F-3111D4E71347}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{D8A2D3F8-70F8-5F46-AFB6-9851AC625006}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{B3162829-A9B5-9B4E-B15E-0C9A5F9AD885}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{7C8AF355-C8D2-2B4A-8537-E4529AC0A8BA}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{6BCE250D-C482-7C4C-ADFB-4E48E27D3C72}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{63D43679-8F7E-DA4E-BCCC-361C10F7D39A}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3" display="example@example.comn"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="E15" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleanup.py: state, zip, and dates complete
</commit_message>
<xml_diff>
--- a/test_files/example2.xlsx
+++ b/test_files/example2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700"/>
+    <workbookView xWindow="0" yWindow="7900" windowWidth="25440" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Adress</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Jan. 25, 1950</t>
   </si>
   <si>
-    <t>Janurary 3 2000</t>
-  </si>
-  <si>
     <t>Feb. 3 1989</t>
   </si>
   <si>
@@ -282,6 +276,111 @@
   </si>
   <si>
     <t>John Smith</t>
+  </si>
+  <si>
+    <t>Address Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Bethlehem</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>Blackwood</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>Titusville</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Deerfield</t>
+  </si>
+  <si>
+    <t>IL.</t>
+  </si>
+  <si>
+    <t>Willingboro</t>
+  </si>
+  <si>
+    <t>nj</t>
+  </si>
+  <si>
+    <t>08046-1123</t>
+  </si>
+  <si>
+    <t>Buford</t>
+  </si>
+  <si>
+    <t>Ga.</t>
+  </si>
+  <si>
+    <t>30518-11</t>
+  </si>
+  <si>
+    <t>Hoffman Estates</t>
+  </si>
+  <si>
+    <t>Il</t>
+  </si>
+  <si>
+    <t>Capitol Heights</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>Mount Juliet</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>30132-1123</t>
+  </si>
+  <si>
+    <t>Middletown</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Cumming</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>Voorhees</t>
+  </si>
+  <si>
+    <t>January 3 2000</t>
   </si>
 </sst>
 </file>
@@ -655,337 +754,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="43.1640625" customWidth="1"/>
-    <col min="6" max="6" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" customWidth="1"/>
+    <col min="8" max="8" width="43.1640625" customWidth="1"/>
+    <col min="9" max="9" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2">
+        <v>18015</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3">
+        <v>7202</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4">
+        <v>8012</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="2">
+        <v>31056</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5">
+        <v>32780</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2">
+        <v>34647</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6">
+        <v>60015</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G7" s="2">
+        <v>31056</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9">
+        <v>60169</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="5">
+        <v>34981</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10">
+        <v>20743</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="2">
+        <v>36892</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11">
+        <v>37122</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="2">
+        <v>34489</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12">
+        <v>1714244999</v>
+      </c>
+      <c r="G12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13">
+        <v>6457</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14">
+        <v>30040</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="2">
-        <v>31056</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="2">
-        <v>34647</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="2">
-        <v>31056</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="5">
-        <v>34981</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="2">
-        <v>36892</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2">
-        <v>34489</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>1714244999</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="4" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15">
+        <v>8043</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="5">
+        <v>28216</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="I15" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="5">
-        <v>28216</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3" display="example@example.comn"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E15" r:id="rId13"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3" display="example@example.comn"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="H8" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H11" r:id="rId10"/>
+    <hyperlink ref="H12" r:id="rId11"/>
+    <hyperlink ref="H13" r:id="rId12"/>
+    <hyperlink ref="H15" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleanup.py: web addresses, check against list, and char limit complete
</commit_message>
<xml_diff>
--- a/test_files/example2.xlsx
+++ b/test_files/example2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7900" windowWidth="25440" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -381,6 +381,102 @@
   </si>
   <si>
     <t>January 3 2000</t>
+  </si>
+  <si>
+    <t>Web Address</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>T-Shirt Sizes</t>
+  </si>
+  <si>
+    <t>Favorite Candy</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>www.mysite.com</t>
+  </si>
+  <si>
+    <t>http://mywebsite.com</t>
+  </si>
+  <si>
+    <t>http://www.mywebsite.com</t>
+  </si>
+  <si>
+    <t>https://www.thisisawebsite.com</t>
+  </si>
+  <si>
+    <t>https://thisisawebsite.org</t>
+  </si>
+  <si>
+    <t>://www.thisisnotawebsite.org</t>
+  </si>
+  <si>
+    <t>thisisanotherwebsite.org</t>
+  </si>
+  <si>
+    <t>http://www.thisisyetanotherwebsite.edu</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t>XXL</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Snickers</t>
+  </si>
+  <si>
+    <t>Hershey's Chocolate</t>
+  </si>
+  <si>
+    <t>Kit-Kat</t>
+  </si>
+  <si>
+    <t>Resees</t>
+  </si>
+  <si>
+    <t>Skittles</t>
+  </si>
+  <si>
+    <t>Swedish Fish</t>
+  </si>
+  <si>
+    <t>Butterfinger</t>
+  </si>
+  <si>
+    <t>This is a very long note that will need to be truncated.</t>
+  </si>
+  <si>
+    <t>This is a note.</t>
   </si>
 </sst>
 </file>
@@ -754,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -770,10 +866,14 @@
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
     <col min="7" max="7" width="27.1640625" customWidth="1"/>
     <col min="8" max="8" width="43.1640625" customWidth="1"/>
-    <col min="9" max="9" width="28.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,8 +901,23 @@
       <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -830,8 +945,20 @@
       <c r="I2" t="s">
         <v>51</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N2" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -859,8 +986,20 @@
       <c r="I3" t="s">
         <v>59</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M3" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -888,8 +1027,17 @@
       <c r="I4" t="s">
         <v>52</v>
       </c>
+      <c r="J4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M4" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -917,8 +1065,15 @@
       <c r="I5" t="s">
         <v>55</v>
       </c>
+      <c r="J5" s="4"/>
+      <c r="L5" t="s">
+        <v>131</v>
+      </c>
+      <c r="M5" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -946,8 +1101,17 @@
       <c r="I6" t="s">
         <v>56</v>
       </c>
+      <c r="J6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="L6" t="s">
+        <v>132</v>
+      </c>
+      <c r="M6" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -975,8 +1139,20 @@
       <c r="I7" t="s">
         <v>57</v>
       </c>
+      <c r="J7" t="s">
+        <v>125</v>
+      </c>
+      <c r="L7" t="s">
+        <v>133</v>
+      </c>
+      <c r="M7" t="s">
+        <v>141</v>
+      </c>
+      <c r="N7" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1004,8 +1180,14 @@
       <c r="I8" t="s">
         <v>58</v>
       </c>
+      <c r="L8" t="s">
+        <v>134</v>
+      </c>
+      <c r="M8" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1033,8 +1215,17 @@
       <c r="I9" t="s">
         <v>60</v>
       </c>
+      <c r="J9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" t="s">
+        <v>135</v>
+      </c>
+      <c r="M9" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1062,8 +1253,17 @@
       <c r="I10" t="s">
         <v>61</v>
       </c>
+      <c r="L10" t="s">
+        <v>136</v>
+      </c>
+      <c r="M10" t="s">
+        <v>138</v>
+      </c>
+      <c r="N10" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1091,8 +1291,14 @@
       <c r="I11" t="s">
         <v>62</v>
       </c>
+      <c r="L11" t="s">
+        <v>130</v>
+      </c>
+      <c r="M11" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1120,8 +1326,17 @@
       <c r="I12" s="6" t="s">
         <v>63</v>
       </c>
+      <c r="J12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L12" t="s">
+        <v>129</v>
+      </c>
+      <c r="M12" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1149,8 +1364,14 @@
       <c r="I13" t="s">
         <v>64</v>
       </c>
+      <c r="L13" t="s">
+        <v>128</v>
+      </c>
+      <c r="M13" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1178,8 +1399,17 @@
       <c r="I14" t="s">
         <v>53</v>
       </c>
+      <c r="J14" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="L14" t="s">
+        <v>137</v>
+      </c>
+      <c r="M14" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1223,6 +1453,12 @@
     <hyperlink ref="H12" r:id="rId11"/>
     <hyperlink ref="H13" r:id="rId12"/>
     <hyperlink ref="H15" r:id="rId13"/>
+    <hyperlink ref="J2" r:id="rId14"/>
+    <hyperlink ref="J3" r:id="rId15"/>
+    <hyperlink ref="J4" r:id="rId16"/>
+    <hyperlink ref="J6" r:id="rId17"/>
+    <hyperlink ref="J9" r:id="rId18"/>
+    <hyperlink ref="J14" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleanup.py: All but social media complete
</commit_message>
<xml_diff>
--- a/test_files/example2.xlsx
+++ b/test_files/example2.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -477,12 +477,27 @@
   </si>
   <si>
     <t>This is a note.</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Satisfaction Rate</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -527,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -535,6 +550,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -850,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,10 +886,12 @@
     <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -914,10 +932,16 @@
         <v>118</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -954,11 +978,17 @@
       <c r="M2" t="s">
         <v>138</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2" s="7">
+        <v>621</v>
+      </c>
+      <c r="P2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -995,11 +1025,17 @@
       <c r="M3" t="s">
         <v>139</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>5296</v>
+      </c>
+      <c r="P3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1036,8 +1072,14 @@
       <c r="M4" t="s">
         <v>138</v>
       </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4" s="7">
+        <v>8488.23</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1072,8 +1114,14 @@
       <c r="M5" t="s">
         <v>140</v>
       </c>
+      <c r="N5">
+        <v>3.2</v>
+      </c>
+      <c r="O5">
+        <v>7568.23</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1110,8 +1158,14 @@
       <c r="M6" t="s">
         <v>141</v>
       </c>
+      <c r="N6">
+        <v>4.5</v>
+      </c>
+      <c r="O6" s="7">
+        <v>6419.56</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1148,11 +1202,17 @@
       <c r="M7" t="s">
         <v>141</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7">
+        <v>2.5</v>
+      </c>
+      <c r="O7">
+        <v>3564</v>
+      </c>
+      <c r="P7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1186,8 +1246,14 @@
       <c r="M8" t="s">
         <v>142</v>
       </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8" s="7">
+        <v>7720</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1224,8 +1290,14 @@
       <c r="M9" t="s">
         <v>143</v>
       </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>1015</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1259,11 +1331,17 @@
       <c r="M10" t="s">
         <v>138</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>7363.23</v>
+      </c>
+      <c r="P10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1297,8 +1375,14 @@
       <c r="M11" t="s">
         <v>144</v>
       </c>
+      <c r="N11" t="s">
+        <v>149</v>
+      </c>
+      <c r="O11" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1335,8 +1419,14 @@
       <c r="M12" t="s">
         <v>140</v>
       </c>
+      <c r="N12">
+        <v>3.4</v>
+      </c>
+      <c r="O12">
+        <v>8470.32</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1370,8 +1460,14 @@
       <c r="M13" t="s">
         <v>138</v>
       </c>
+      <c r="N13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O13" s="7">
+        <v>8585</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1408,8 +1504,14 @@
       <c r="M14" t="s">
         <v>141</v>
       </c>
+      <c r="N14">
+        <v>2.7</v>
+      </c>
+      <c r="O14" s="7">
+        <v>2542</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
graph.py: initialize plotting complete
</commit_message>
<xml_diff>
--- a/test_files/example2.xlsx
+++ b/test_files/example2.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -483,12 +483,6 @@
   </si>
   <si>
     <t>Satisfaction Rate</t>
-  </si>
-  <si>
-    <t>One</t>
-  </si>
-  <si>
-    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -869,7 +863,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1375,11 +1369,11 @@
       <c r="M11" t="s">
         <v>144</v>
       </c>
-      <c r="N11" t="s">
-        <v>149</v>
-      </c>
-      <c r="O11" t="s">
-        <v>150</v>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>7363.23</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>